<commit_message>
implementação situação atual arquivo.json
</commit_message>
<xml_diff>
--- a/noticias.xlsx
+++ b/noticias.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,117 +453,108 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>VÍDEO: indígenas comemoram do lado de fora do STF</t>
+          <t>Voto 'sim' de Jaques Wagner causa mal-estar e surpreende o STF</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/df/distrito-federal/noticia/2023/09/21/video-indigenas-comemoram-derrubada-de-marco-temporal-stf-forma-maioria-contra-tese.ghtml</t>
+          <t>https://g1.globo.com/politica/blog/natuza-nery/post/2023/11/23/voto-de-jaques-em-pec-racha-lideranca-do-governo-e-surpreende-ministros.ghtml</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Aras diz em sua despedida da PGR que sofreu com 'falsas narrativas'</t>
+          <t>Hamas vai libertar amanhã 1º grupo de reféns com 13 mulheres e crianças</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/politica/noticia/2023/09/21/em-fim-de-mandato-na-pgr-aras-diz-que-ultimos-anos-tiveram-falsas-narrativas-e-incompreensoes.ghtml</t>
+          <t>https://g1.globo.com/mundo/noticia/2023/11/23/hamas-vai-libertar-13-civis-em-primeiro-grupo-diz-qatar.ghtml</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Cid revela em delação que Bolsonaro consultou militares sobre golpe</t>
+          <t>Polícia encontra casa em SP com 33 pessoas treinadas para engolir drogas</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://oglobo.globo.com/blogs/bela-megale/post/2023/09/em-delacao-mauro-cid-revela-que-bolsonaro-fez-reuniao-com-cupula-militar-para-avaliar-golpe-no-pais.ghtml</t>
+          <t>https://g1.globo.com/sp/sao-paulo/noticia/2023/11/23/homem-e-preso-suspeito-de-aliciar-e-treinar-mais-de-30-pessoas-para-engolir-drogas-e-leva-las-a-europa-grupo-foi-encontrado-com-passaportes-e-cocaina.ghtml</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Múcio diz que ex-chefe da Marinha não estava '100% do lado da lei'</t>
+          <t>Dor terrível e até morte: o que pode acontecer com as 'mulas' do tráfico</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/politica/noticia/2023/09/21/estavamos-100percent-do-lado-da-lei-e-ele-nao-diz-ministro-da-defesa-sobre-ex-comandante-da-marinha-citado-por-cid-em-delacao.ghtml</t>
+          <t>https://g1.globo.com/saude/noticia/2023/11/23/desmaios-dores-terriveis-convulsoes-e-morte-o-que-acontece-no-organismo-de-quem-transporta-drogas-no-estomago-no-reto-ou-na-vagina.ghtml</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>11 capitais devem bater recorde de calor do ano até o fim de semana</t>
+          <t>Celulares top de linha: g1 testa 4 modelos objetos de desejo</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/meio-ambiente/noticia/2023/09/21/recorde-de-temperatura-setembro-capitais.ghtml</t>
+          <t>https://g1.globo.com/guia/guia-de-compras/tecnologia/celulares/celulares-topo-de-linha-g1-testa-4-smartphones-que-sao-objetos-de-desejo.ghtml</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Insolação e golpe de calor: entenda a diferença e veja cuidados</t>
+          <t xml:space="preserve">EUA enviam documentos que comprovam recompra de relógio por advogado de Bolsonaro </t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/saude/noticia/2023/09/21/temperatura-alta-o-que-fazer-em-caso-de-insolacao-e-golpe-de-calor.ghtml</t>
+          <t>https://g1.globo.com/politica/blog/andreia-sadi/post/2023/11/23/pf-recebe-documentos-da-justica-americana-que-comprovam-recompra-de-relogio-de-bolsonaro-nos-eua.ghtml</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Vai ter horário de verão? Área técnica não vê necessidade</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
+          <t>Entenda proposta de federalizar a Cemig para pagar dívidas de MG</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Estado deve R$ 160 bilhões e negocia recuperação fiscal com o governo federal.</t>
+        </is>
+      </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/politica/noticia/2023/09/21/horario-de-verao-area-tecnica-de-minas-e-energia-nao-ve-necessidade-de-retomar-medida-em-2023.ghtml</t>
+          <t>https://g1.globo.com/mg/minas-gerais/noticia/2023/11/23/entenda-a-divida-de-mg-com-a-uniao-o-que-e-o-regime-de-recuperacao-fiscal-e-a-alternativa-que-inclui-federalizacao-da-cemig.ghtml</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Em vídeo, pastor suspeito promete a fiéis ganho com 'tecnologia quântica'</t>
+          <t>Desabamento de prédio, gritos de socorro no mar e mais VÍDEOS do dia</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/df/distrito-federal/noticia/2023/09/21/nesara-gesara-video-mostra-pastor-golpista-explicando-como-vai-pagar-fieis-com-tecnologia-quantica-e-projeto-redencao.ghtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>É rapidinho: vídeo explica como entrar no canal do g1 no WhatsApp</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>https://g1.globo.com/tecnologia/noticia/2023/09/13/g1-canais-whatsapp.ghtml</t>
+          <t>https://g1.globo.com/playlist/videos-para-assistir-agora.ghtml</t>
         </is>
       </c>
     </row>

</xml_diff>